<commit_message>
if holifay and if rain modify
</commit_message>
<xml_diff>
--- a/If_holiday.xlsx
+++ b/If_holiday.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ET\Desktop\機器學習專案\ML\extend_X_feature\holiday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morri\Documents\GitHub\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EDD8EC-AB7D-40FF-8421-E9922731C8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FF63C1-76A4-4EFE-AFF9-2C691D196172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -39,17 +39,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -357,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,7 +373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>20231002</v>
       </c>
@@ -381,7 +381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>20231003</v>
       </c>
@@ -389,7 +389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>20231004</v>
       </c>
@@ -397,7 +397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>20231005</v>
       </c>
@@ -405,7 +405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>20231006</v>
       </c>
@@ -413,7 +413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>20231007</v>
       </c>
@@ -421,7 +421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>20231008</v>
       </c>
@@ -429,7 +429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>20231009</v>
       </c>
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>20231010</v>
       </c>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>20231011</v>
       </c>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>20231012</v>
       </c>
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>20231013</v>
       </c>
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>20231014</v>
       </c>
@@ -477,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>20231015</v>
       </c>
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>20231016</v>
       </c>
@@ -493,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>20231017</v>
       </c>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>20231018</v>
       </c>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>20231019</v>
       </c>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>20231020</v>
       </c>
@@ -525,7 +525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20231021</v>
       </c>
@@ -533,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>20231022</v>
       </c>
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>20231023</v>
       </c>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>20231024</v>
       </c>
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>20231025</v>
       </c>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>20231026</v>
       </c>
@@ -573,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>20231027</v>
       </c>
@@ -581,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>20231028</v>
       </c>
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>20231029</v>
       </c>
@@ -597,7 +597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>20231030</v>
       </c>
@@ -605,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>20231031</v>
       </c>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>20231101</v>
       </c>
@@ -621,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>20231102</v>
       </c>
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>20231103</v>
       </c>
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>20231104</v>
       </c>
@@ -645,7 +645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>20231105</v>
       </c>
@@ -653,7 +653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>20231106</v>
       </c>
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>20231107</v>
       </c>
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>20231108</v>
       </c>
@@ -677,7 +677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>20231109</v>
       </c>
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>20231110</v>
       </c>
@@ -693,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>20231111</v>
       </c>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>20231112</v>
       </c>
@@ -709,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>20231113</v>
       </c>
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>20231114</v>
       </c>
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>20231115</v>
       </c>
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>20231116</v>
       </c>
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>20231117</v>
       </c>
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>20231118</v>
       </c>
@@ -757,7 +757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>20231119</v>
       </c>
@@ -765,7 +765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>20231120</v>
       </c>
@@ -773,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>20231121</v>
       </c>
@@ -781,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>20231122</v>
       </c>
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>20231123</v>
       </c>
@@ -797,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>20231124</v>
       </c>
@@ -805,7 +805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>20231125</v>
       </c>
@@ -813,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>20231126</v>
       </c>
@@ -821,7 +821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>20231127</v>
       </c>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>20231128</v>
       </c>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>20231129</v>
       </c>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>20231130</v>
       </c>
@@ -853,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>20231201</v>
       </c>
@@ -861,7 +861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>20231202</v>
       </c>
@@ -869,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>20231203</v>
       </c>
@@ -877,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>20231204</v>
       </c>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>20231205</v>
       </c>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>20231206</v>
       </c>
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>20231207</v>
       </c>
@@ -909,12 +909,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>20231208</v>
       </c>
       <c r="B69">
         <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>20231209</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>